<commit_message>
new updates regarding pass test case
new updates regarding pass test case
</commit_message>
<xml_diff>
--- a/lib_template/com.microsite.runner.xlsx
+++ b/lib_template/com.microsite.runner.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="MicroSiteRunner" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="MicroSiteRunner" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="97">
   <si>
     <t>S.No</t>
   </si>
@@ -312,6 +312,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,55 +383,55 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="10" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -447,10 +448,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -485,7 +486,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -520,7 +521,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -608,7 +609,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -617,13 +618,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -633,7 +634,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -642,7 +643,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -651,7 +652,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -661,12 +662,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -697,7 +698,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -716,7 +717,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -728,22 +729,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -783,55 +784,410 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row ht="30" r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row ht="30" r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="D13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="14" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1184,7 +1540,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -1408,7 +1764,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>14</v>
       </c>
@@ -1538,18 +1894,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
-    <hyperlink ref="C9" r:id="rId3"/>
-    <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="C5" r:id="rId6"/>
-    <hyperlink ref="C11" r:id="rId7"/>
-    <hyperlink ref="C3" r:id="rId8"/>
-    <hyperlink ref="C2" r:id="rId9"/>
-    <hyperlink ref="C15" r:id="rId10"/>
+    <hyperlink r:id="rId1" ref="C7"/>
+    <hyperlink r:id="rId2" ref="C8"/>
+    <hyperlink r:id="rId3" ref="C9"/>
+    <hyperlink r:id="rId4" ref="C10"/>
+    <hyperlink r:id="rId5" ref="C4"/>
+    <hyperlink r:id="rId6" ref="C5"/>
+    <hyperlink r:id="rId7" ref="C11"/>
+    <hyperlink r:id="rId8" ref="C3"/>
+    <hyperlink r:id="rId9" ref="C2"/>
+    <hyperlink r:id="rId10" ref="C15"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new folder for screenshot
new folder for screenshot
</commit_message>
<xml_diff>
--- a/lib_template/com.microsite.runner.xlsx
+++ b/lib_template/com.microsite.runner.xlsx
@@ -1026,7 +1026,7 @@
         <v>37</v>
       </c>
       <c r="H9" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>68</v>
@@ -1058,7 +1058,7 @@
         <v>37</v>
       </c>
       <c r="H10" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>68</v>
@@ -1090,7 +1090,7 @@
         <v>37</v>
       </c>
       <c r="H11" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
delete jar and update runner
delete jar and update runner
</commit_message>
<xml_diff>
--- a/lib_template/com.microsite.runner.xlsx
+++ b/lib_template/com.microsite.runner.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="MicroSiteRunner" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
+    <sheet name="MicroSiteRunner" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="127">
   <si>
     <t>S.No</t>
   </si>
@@ -402,7 +402,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,59 +472,59 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="10" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -542,10 +541,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -580,7 +579,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,7 +614,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,7 +702,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -712,13 +711,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -728,7 +727,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -737,7 +736,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -746,7 +745,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -756,12 +755,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -792,7 +791,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -811,7 +810,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -823,22 +822,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -877,14 +876,14 @@
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>97</v>
+      <c r="B2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>90</v>
@@ -896,337 +895,40 @@
         <v>37</v>
       </c>
       <c r="H2" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
-    <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" ref="C5"/>
-    <hyperlink r:id="rId5" ref="C6"/>
-    <hyperlink r:id="rId6" ref="C7"/>
-    <hyperlink r:id="rId7" ref="C8"/>
-    <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C10"/>
-    <hyperlink r:id="rId10" ref="C11"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J26"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1579,7 +1281,7 @@
         <v>70</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -1803,7 +1505,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="30" r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>14</v>
       </c>
@@ -1931,20 +1633,382 @@
         <v>94</v>
       </c>
     </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C7"/>
-    <hyperlink r:id="rId2" ref="C8"/>
-    <hyperlink r:id="rId3" ref="C9"/>
-    <hyperlink r:id="rId4" ref="C10"/>
-    <hyperlink r:id="rId5" ref="C4"/>
-    <hyperlink r:id="rId6" ref="C5"/>
-    <hyperlink r:id="rId7" ref="C11"/>
-    <hyperlink r:id="rId8" ref="C3"/>
-    <hyperlink r:id="rId9" ref="C2"/>
-    <hyperlink r:id="rId10" ref="C15"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="C2" r:id="rId9"/>
+    <hyperlink ref="C15" r:id="rId10"/>
+    <hyperlink ref="C29" r:id="rId11"/>
+    <hyperlink ref="C30" r:id="rId12"/>
+    <hyperlink ref="C31" r:id="rId13"/>
+    <hyperlink ref="C32" r:id="rId14"/>
+    <hyperlink ref="C33" r:id="rId15"/>
+    <hyperlink ref="C34" r:id="rId16"/>
+    <hyperlink ref="C35" r:id="rId17"/>
+    <hyperlink ref="C36" r:id="rId18"/>
+    <hyperlink ref="C37" r:id="rId19"/>
+    <hyperlink ref="C38" r:id="rId20"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new jar and runner file updates
new jar and runner file updates
</commit_message>
<xml_diff>
--- a/lib_template/com.microsite.runner.xlsx
+++ b/lib_template/com.microsite.runner.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="MicroSiteRunner" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
+    <sheet name="MicroSiteRunner" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="127">
   <si>
     <t>S.No</t>
   </si>
@@ -402,7 +402,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,59 +472,59 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="10" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -542,10 +541,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -580,7 +579,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,7 +614,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,7 +702,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -712,13 +711,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -728,7 +727,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -737,7 +736,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -746,7 +745,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -756,12 +755,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -792,7 +791,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -811,7 +810,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -823,22 +822,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -877,59 +876,356 @@
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="19" t="s">
+      <c r="E11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1282,7 +1578,7 @@
         <v>70</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1802,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="30" r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>14</v>
       </c>
@@ -1988,28 +2284,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C7"/>
-    <hyperlink r:id="rId2" ref="C8"/>
-    <hyperlink r:id="rId3" ref="C9"/>
-    <hyperlink r:id="rId4" ref="C10"/>
-    <hyperlink r:id="rId5" ref="C4"/>
-    <hyperlink r:id="rId6" ref="C5"/>
-    <hyperlink r:id="rId7" ref="C11"/>
-    <hyperlink r:id="rId8" ref="C3"/>
-    <hyperlink r:id="rId9" ref="C2"/>
-    <hyperlink r:id="rId10" ref="C15"/>
-    <hyperlink r:id="rId11" ref="C29"/>
-    <hyperlink r:id="rId12" ref="C30"/>
-    <hyperlink r:id="rId13" ref="C31"/>
-    <hyperlink r:id="rId14" ref="C32"/>
-    <hyperlink r:id="rId15" ref="C33"/>
-    <hyperlink r:id="rId16" ref="C34"/>
-    <hyperlink r:id="rId17" ref="C35"/>
-    <hyperlink r:id="rId18" ref="C36"/>
-    <hyperlink r:id="rId19" ref="C37"/>
-    <hyperlink r:id="rId20" ref="C38"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="C2" r:id="rId9"/>
+    <hyperlink ref="C15" r:id="rId10"/>
+    <hyperlink ref="C29" r:id="rId11"/>
+    <hyperlink ref="C30" r:id="rId12"/>
+    <hyperlink ref="C31" r:id="rId13"/>
+    <hyperlink ref="C32" r:id="rId14"/>
+    <hyperlink ref="C33" r:id="rId15"/>
+    <hyperlink ref="C34" r:id="rId16"/>
+    <hyperlink ref="C35" r:id="rId17"/>
+    <hyperlink ref="C36" r:id="rId18"/>
+    <hyperlink ref="C37" r:id="rId19"/>
+    <hyperlink ref="C38" r:id="rId20"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>